<commit_message>
edit the loop that read from xlcsx file
</commit_message>
<xml_diff>
--- a/ConsoleApp1/Employe list.xlsx
+++ b/ConsoleApp1/Employe list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yasmeen's files\ConsoleApp1\ConsoleApp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B928C52-CF4B-4C46-9DC6-0ADD67862278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33E482-CF4F-4C0D-8137-0B8B6386BB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4065" yWindow="3930" windowWidth="18000" windowHeight="10875" xr2:uid="{7E72585A-307E-43AE-ADD6-F1CB4FC42337}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
check if the row exist before inserting
</commit_message>
<xml_diff>
--- a/ConsoleApp1/Employe list.xlsx
+++ b/ConsoleApp1/Employe list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yasmeen's files\ConsoleApp1\ConsoleApp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33E482-CF4F-4C0D-8137-0B8B6386BB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930048F5-0B9E-4C8C-A3C0-2C0A2DE1603F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4065" yWindow="3930" windowWidth="18000" windowHeight="10875" xr2:uid="{7E72585A-307E-43AE-ADD6-F1CB4FC42337}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Employee name</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>0112548988482</t>
+  </si>
+  <si>
+    <t>yasmeen  ahmed</t>
   </si>
 </sst>
 </file>
@@ -498,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441B52D7-D099-4ACF-B2B5-27DFC41220C9}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +681,36 @@
         <v>33</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <v>2351</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7" si="1">F7*1.25</f>
+        <v>2938.75</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{67BFD072-9DF9-40B7-9100-CF1D759970A2}"/>
@@ -682,6 +718,7 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{E45A73D2-3E26-405E-B35A-C6D20880259D}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{2D1CA878-2D3B-46CD-83C1-E501D5A7210A}"/>
     <hyperlink ref="D5" r:id="rId5" xr:uid="{FC9F04FB-F3F1-4D4E-9CDB-A211E174605D}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{5E71F50F-05EF-4B44-A680-11AD8BECF2D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>